<commit_message>
exp 3 node fix applied
</commit_message>
<xml_diff>
--- a/Experiment 3/Trace Files/LatencyGraph.xlsx
+++ b/Experiment 3/Trace Files/LatencyGraph.xlsx
@@ -268,61 +268,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>22.259603603599999</c:v>
+                  <c:v>73.680941176499999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.8623298539</c:v>
+                  <c:v>64.992000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.242212766000002</c:v>
+                  <c:v>67.248000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.922349007299999</c:v>
+                  <c:v>65.361999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.9290733753</c:v>
+                  <c:v>65.37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.922349007299999</c:v>
+                  <c:v>65.335999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.921573221799999</c:v>
+                  <c:v>65.325999999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.9180020899</c:v>
+                  <c:v>65.31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.916217573200001</c:v>
+                  <c:v>65.293999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.915769633499998</c:v>
+                  <c:v>65.286000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.910861924700001</c:v>
+                  <c:v>65.262</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.9103113898</c:v>
+                  <c:v>65.254000000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.908425887300002</c:v>
+                  <c:v>65.248000000000005</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.909403141399999</c:v>
+                  <c:v>65.249610062900004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.907636363600002</c:v>
+                  <c:v>65.249610062900004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20.907636363600002</c:v>
+                  <c:v>65.241559748399993</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.9085188285</c:v>
+                  <c:v>65.249610062900004</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.907636363600002</c:v>
+                  <c:v>65.249610062900004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.224</c:v>
+                  <c:v>65.248000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -428,55 +428,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="2">
-                  <c:v>21.984071588399999</c:v>
+                  <c:v>44.356094276100002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.750788912600001</c:v>
+                  <c:v>43.651884983999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.741455709699999</c:v>
+                  <c:v>43.6248205128</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.7415778252</c:v>
+                  <c:v>43.624281150199998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.741387406600001</c:v>
+                  <c:v>43.624615384599998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.7412366738</c:v>
+                  <c:v>43.623258785899999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.740704375699998</c:v>
+                  <c:v>43.622564102600002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.7415778252</c:v>
+                  <c:v>43.624281150199998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.741045891100001</c:v>
+                  <c:v>43.6235897436</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.7395309168</c:v>
+                  <c:v>43.618146964899999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.742222222199999</c:v>
+                  <c:v>43.626666666699997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.741767838099999</c:v>
+                  <c:v>43.625303514400002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.742222222199999</c:v>
+                  <c:v>43.626666666699997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.741767838099999</c:v>
+                  <c:v>43.625303514400002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.742070437599999</c:v>
+                  <c:v>43.626666666699997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.741918976499999</c:v>
+                  <c:v>43.625303514400002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>21.6</c:v>
+                  <c:v>43.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,11 +492,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-104742480"/>
-        <c:axId val="-104734864"/>
+        <c:axId val="193698320"/>
+        <c:axId val="193706480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-104742480"/>
+        <c:axId val="193698320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104734864"/>
+        <c:crossAx val="193706480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -608,7 +608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-104734864"/>
+        <c:axId val="193706480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
@@ -716,7 +716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104742480"/>
+        <c:crossAx val="193698320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -972,61 +972,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>22.259603603599999</c:v>
+                  <c:v>73.680941176499999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.8623298539</c:v>
+                  <c:v>64.992000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.257751772999999</c:v>
+                  <c:v>67.444313725499995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.158678678699999</c:v>
+                  <c:v>66.4769655172</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.262222222199998</c:v>
+                  <c:v>67.054159291999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.980673774</c:v>
+                  <c:v>65.766233766200003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.9236865204</c:v>
+                  <c:v>65.356276729599998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.919455497400001</c:v>
+                  <c:v>65.342379746800006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.918336468100001</c:v>
+                  <c:v>65.316025157200002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.916217573200001</c:v>
+                  <c:v>65.316025157200002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.910861924700001</c:v>
+                  <c:v>65.281999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.910861924700001</c:v>
+                  <c:v>65.283823899400005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.905964472299999</c:v>
+                  <c:v>65.259672956000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.904626959200002</c:v>
+                  <c:v>65.251622641500006</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.905085594999999</c:v>
+                  <c:v>65.249610062900004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20.903036649200001</c:v>
+                  <c:v>65.241559748399993</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.905964472299999</c:v>
+                  <c:v>65.249610062900004</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.905964472299999</c:v>
+                  <c:v>65.249610062900004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.7150344828</c:v>
+                  <c:v>65.293176470600002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1132,55 +1132,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="2">
-                  <c:v>21.698426008999999</c:v>
+                  <c:v>43.496608108099998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.6951130064</c:v>
+                  <c:v>43.485035143799998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.884269518699998</c:v>
+                  <c:v>44.051897435900003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.783761702100001</c:v>
+                  <c:v>43.751872204500003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.7367521368</c:v>
+                  <c:v>43.610256410300003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.7390415335</c:v>
+                  <c:v>43.6171246006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.736811099299999</c:v>
+                  <c:v>43.6108717949</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.738371002099999</c:v>
+                  <c:v>43.614670926499997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.7434529915</c:v>
+                  <c:v>43.630358974400004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.7378828541</c:v>
+                  <c:v>43.6136485623</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.741059829099999</c:v>
+                  <c:v>43.623179487199998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.7406091587</c:v>
+                  <c:v>43.621827476</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.7396923077</c:v>
+                  <c:v>43.619076923100003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.743335463299999</c:v>
+                  <c:v>43.630006389800002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.7395432231</c:v>
+                  <c:v>43.619076923100003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.7415923159</c:v>
+                  <c:v>43.625230769200002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>21.610643923200001</c:v>
+                  <c:v>43.231897763600003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1196,11 +1196,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-104731600"/>
-        <c:axId val="-104741936"/>
+        <c:axId val="193699408"/>
+        <c:axId val="193705392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-104731600"/>
+        <c:axId val="193699408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1304,7 +1304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104741936"/>
+        <c:crossAx val="193705392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1312,7 +1312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-104741936"/>
+        <c:axId val="193705392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
@@ -1420,7 +1420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104731600"/>
+        <c:crossAx val="193699408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2946,7 +2946,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="D3" sqref="D3:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
@@ -2981,10 +2981,10 @@
         <v>0.5</v>
       </c>
       <c r="B3">
-        <v>22.259603603599999</v>
+        <v>73.680941176499999</v>
       </c>
       <c r="D3">
-        <v>22.259603603599999</v>
+        <v>73.680941176499999</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2992,10 +2992,10 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>20.8623298539</v>
+        <v>64.992000000000004</v>
       </c>
       <c r="D4">
-        <v>20.8623298539</v>
+        <v>64.992000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3003,16 +3003,16 @@
         <v>1.5</v>
       </c>
       <c r="B5">
-        <v>21.242212766000002</v>
+        <v>67.248000000000005</v>
       </c>
       <c r="C5">
-        <v>21.984071588399999</v>
+        <v>44.356094276100002</v>
       </c>
       <c r="D5">
-        <v>21.257751772999999</v>
+        <v>67.444313725499995</v>
       </c>
       <c r="E5">
-        <v>21.698426008999999</v>
+        <v>43.496608108099998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -3020,16 +3020,16 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>20.922349007299999</v>
+        <v>65.361999999999995</v>
       </c>
       <c r="C6">
-        <v>21.750788912600001</v>
+        <v>43.651884983999999</v>
       </c>
       <c r="D6">
-        <v>21.158678678699999</v>
+        <v>66.4769655172</v>
       </c>
       <c r="E6">
-        <v>21.6951130064</v>
+        <v>43.485035143799998</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3037,16 +3037,16 @@
         <v>2.5</v>
       </c>
       <c r="B7">
-        <v>20.9290733753</v>
+        <v>65.37</v>
       </c>
       <c r="C7">
-        <v>21.741455709699999</v>
+        <v>43.6248205128</v>
       </c>
       <c r="D7">
-        <v>21.262222222199998</v>
+        <v>67.054159291999994</v>
       </c>
       <c r="E7">
-        <v>21.884269518699998</v>
+        <v>44.051897435900003</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3054,16 +3054,16 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>20.922349007299999</v>
+        <v>65.335999999999999</v>
       </c>
       <c r="C8">
-        <v>21.7415778252</v>
+        <v>43.624281150199998</v>
       </c>
       <c r="D8">
-        <v>20.980673774</v>
+        <v>65.766233766200003</v>
       </c>
       <c r="E8">
-        <v>21.783761702100001</v>
+        <v>43.751872204500003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3071,16 +3071,16 @@
         <v>3.5</v>
       </c>
       <c r="B9">
-        <v>20.921573221799999</v>
+        <v>65.325999999999993</v>
       </c>
       <c r="C9">
-        <v>21.741387406600001</v>
+        <v>43.624615384599998</v>
       </c>
       <c r="D9">
-        <v>20.9236865204</v>
+        <v>65.356276729599998</v>
       </c>
       <c r="E9">
-        <v>21.7367521368</v>
+        <v>43.610256410300003</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -3088,16 +3088,16 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>20.9180020899</v>
+        <v>65.31</v>
       </c>
       <c r="C10">
-        <v>21.7412366738</v>
+        <v>43.623258785899999</v>
       </c>
       <c r="D10">
-        <v>20.919455497400001</v>
+        <v>65.342379746800006</v>
       </c>
       <c r="E10">
-        <v>21.7390415335</v>
+        <v>43.6171246006</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -3105,16 +3105,16 @@
         <v>4.5</v>
       </c>
       <c r="B11">
-        <v>20.916217573200001</v>
+        <v>65.293999999999997</v>
       </c>
       <c r="C11">
-        <v>21.740704375699998</v>
+        <v>43.622564102600002</v>
       </c>
       <c r="D11">
-        <v>20.918336468100001</v>
+        <v>65.316025157200002</v>
       </c>
       <c r="E11">
-        <v>21.736811099299999</v>
+        <v>43.6108717949</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -3122,16 +3122,16 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>20.915769633499998</v>
+        <v>65.286000000000001</v>
       </c>
       <c r="C12">
-        <v>21.7415778252</v>
+        <v>43.624281150199998</v>
       </c>
       <c r="D12">
-        <v>20.916217573200001</v>
+        <v>65.316025157200002</v>
       </c>
       <c r="E12">
-        <v>21.738371002099999</v>
+        <v>43.614670926499997</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -3139,16 +3139,16 @@
         <v>5.5</v>
       </c>
       <c r="B13">
-        <v>20.910861924700001</v>
+        <v>65.262</v>
       </c>
       <c r="C13">
-        <v>21.741045891100001</v>
+        <v>43.6235897436</v>
       </c>
       <c r="D13">
-        <v>20.910861924700001</v>
+        <v>65.281999999999996</v>
       </c>
       <c r="E13">
-        <v>21.7434529915</v>
+        <v>43.630358974400004</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -3156,16 +3156,16 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>20.9103113898</v>
+        <v>65.254000000000005</v>
       </c>
       <c r="C14">
-        <v>21.7395309168</v>
+        <v>43.618146964899999</v>
       </c>
       <c r="D14">
-        <v>20.910861924700001</v>
+        <v>65.283823899400005</v>
       </c>
       <c r="E14">
-        <v>21.7378828541</v>
+        <v>43.6136485623</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -3173,16 +3173,16 @@
         <v>6.5</v>
       </c>
       <c r="B15">
-        <v>20.908425887300002</v>
+        <v>65.248000000000005</v>
       </c>
       <c r="C15">
-        <v>21.742222222199999</v>
+        <v>43.626666666699997</v>
       </c>
       <c r="D15">
-        <v>20.905964472299999</v>
+        <v>65.259672956000003</v>
       </c>
       <c r="E15">
-        <v>21.741059829099999</v>
+        <v>43.623179487199998</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -3190,16 +3190,16 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <v>20.909403141399999</v>
+        <v>65.249610062900004</v>
       </c>
       <c r="C16">
-        <v>21.741767838099999</v>
+        <v>43.625303514400002</v>
       </c>
       <c r="D16">
-        <v>20.904626959200002</v>
+        <v>65.251622641500006</v>
       </c>
       <c r="E16">
-        <v>21.7406091587</v>
+        <v>43.621827476</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -3207,16 +3207,16 @@
         <v>7.5</v>
       </c>
       <c r="B17">
-        <v>20.907636363600002</v>
+        <v>65.249610062900004</v>
       </c>
       <c r="C17">
-        <v>21.742222222199999</v>
+        <v>43.626666666699997</v>
       </c>
       <c r="D17">
-        <v>20.905085594999999</v>
+        <v>65.249610062900004</v>
       </c>
       <c r="E17">
-        <v>21.7396923077</v>
+        <v>43.619076923100003</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -3224,16 +3224,16 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>20.907636363600002</v>
+        <v>65.241559748399993</v>
       </c>
       <c r="C18">
-        <v>21.741767838099999</v>
+        <v>43.625303514400002</v>
       </c>
       <c r="D18">
-        <v>20.903036649200001</v>
+        <v>65.241559748399993</v>
       </c>
       <c r="E18">
-        <v>21.743335463299999</v>
+        <v>43.630006389800002</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3241,16 +3241,16 @@
         <v>8.5</v>
       </c>
       <c r="B19">
-        <v>20.9085188285</v>
+        <v>65.249610062900004</v>
       </c>
       <c r="C19">
-        <v>21.742070437599999</v>
+        <v>43.626666666699997</v>
       </c>
       <c r="D19">
-        <v>20.905964472299999</v>
+        <v>65.249610062900004</v>
       </c>
       <c r="E19">
-        <v>21.7395432231</v>
+        <v>43.619076923100003</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -3258,16 +3258,16 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>20.907636363600002</v>
+        <v>65.249610062900004</v>
       </c>
       <c r="C20">
-        <v>21.741918976499999</v>
+        <v>43.625303514400002</v>
       </c>
       <c r="D20">
-        <v>20.905964472299999</v>
+        <v>65.249610062900004</v>
       </c>
       <c r="E20">
-        <v>21.7415923159</v>
+        <v>43.625230769200002</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -3275,16 +3275,16 @@
         <v>9.5</v>
       </c>
       <c r="B21">
-        <v>20.224</v>
+        <v>65.248000000000005</v>
       </c>
       <c r="C21">
-        <v>21.6</v>
+        <v>43.2</v>
       </c>
       <c r="D21">
-        <v>20.7150344828</v>
+        <v>65.293176470600002</v>
       </c>
       <c r="E21">
-        <v>21.610643923200001</v>
+        <v>43.231897763600003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>